<commit_message>
Update Excel guides to v1120.0 with LIGHT/FULL version information
Updated both EN and KR process guides:

Changes:
- Version updated: v1118.6 → v1120.0 (Phase 3.0)
- Added "Installation Versions" section explaining LIGHT vs FULL
- Added version-specific StrOrigin Analysis behavior:

  LIGHT Version:
  • Punctuation/Space only: "Punctuation/Space Change"
  • Content changed: "Content Change"

  FULL Version (with BERT AI):
  • Punctuation/Space only: "Punctuation/Space Change"
  • Content changed: Similarity % (e.g., "94.5% similar")

Korean guide (VRS_Manager_Process_Guide_KR.xlsx):
- Same updates in Korean language
- Sheet names: 개요, 기술 참고사항

Both guides now accurately reflect the dual-version architecture
and explain how StrOrigin Analysis behaves in each version.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_KR.xlsx
+++ b/docs/VRS_Manager_Process_Guide_KR.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -81,6 +81,10 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="12">
@@ -163,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +226,9 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -587,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C237"/>
+  <dimension ref="A1:C241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,9 +617,9 @@
       <c r="C1" s="2" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
-        <is>
-          <t>버전 1118.6 (Dict 오류 수정 + 포괄적 테스팅)</t>
+      <c r="A2" s="28" t="inlineStr">
+        <is>
+          <t>Version 1120.0 (Phase 3.0 - 전문 설치 프로그램 시스템)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -647,87 +654,83 @@
       <c r="C6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="14" t="inlineStr">
+        <is>
+          <t>설치 버전</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>VRS Manager는 두 가지 버전으로 제공됩니다:</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • LIGHT 버전 (~150MB): 핵심 기능 포함, 빠른 설치. StrOrigin 분석은 "구두점/공백 변경" 또는 "내용 변경" 표시</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FULL 버전 (~2.6GB): 한국어 BERT 모델 기반 AI 의미 유사도 분석 포함. StrOrigin은 상세한 유사도 백분율 표시 (예: "94.5% similar", "48.2% similar")</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>다양한 버전의 음성 데이터를 비교하고, 번역 작업을 지능적으로 병합하며,</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr"/>
-      <c r="C7" s="2" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>여러 언어 버전에 걸쳐 연속성을 유지할 수 있도록 도와줍니다.</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr"/>
-      <c r="C8" s="2" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr"/>
-      <c r="B9" s="2" t="inlineStr"/>
-      <c r="C9" s="2" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>네 가지 핵심 프로세스</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr"/>
-      <c r="C10" s="2" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr"/>
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>1. Raw Process (원본 비교 프로세스)</t>
+          <t>여러 언어 버전에 걸쳐 연속성을 유지할 수 있도록 도와줍니다.</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   목적: PREVIOUS와 CURRENT 파일을 비교하여 변경사항 감지</t>
-        </is>
-      </c>
+      <c r="A13" s="2" t="inlineStr"/>
       <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   사용 시점: 개발팀에서 새로운 데이터를 받았을 때 변경사항 검토</t>
+          <t>네 가지 핵심 프로세스</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr"/>
       <c r="C14" s="2" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   출력물: 상세한 변경 분류가 포함된 비교 리포트</t>
-        </is>
-      </c>
+      <c r="A15" s="2" t="inlineStr"/>
       <c r="B15" s="2" t="inlineStr"/>
       <c r="C15" s="2" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr"/>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>1. Raw Process (원본 비교 프로세스)</t>
+        </is>
+      </c>
       <c r="B16" s="2" t="inlineStr"/>
       <c r="C16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>2. Working Process (작업 프로세스)</t>
+          <t xml:space="preserve">   목적: PREVIOUS와 CURRENT 파일을 비교하여 변경사항 감지</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr"/>
@@ -736,7 +739,7 @@
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   목적: 지능적인 로직을 사용하여 이전 작업을 새 베이스라인에 가져오기</t>
+          <t xml:space="preserve">   사용 시점: 개발팀에서 새로운 데이터를 받았을 때 변경사항 검토</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr"/>
@@ -745,30 +748,30 @@
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   사용 시점: 완료된 번역을 보존하는 작업 파일 준비가 필요할 때</t>
+          <t xml:space="preserve">   출력물: 상세한 변경 분류가 포함된 비교 리포트</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr"/>
       <c r="C19" s="2" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   출력물: 번역 작업이 가능한 Work Transform 파일</t>
-        </is>
-      </c>
+      <c r="A20" s="2" t="inlineStr"/>
       <c r="B20" s="2" t="inlineStr"/>
       <c r="C20" s="2" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="inlineStr"/>
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2. Working Process (작업 프로세스)</t>
+        </is>
+      </c>
       <c r="B21" s="2" t="inlineStr"/>
       <c r="C21" s="2" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>3. All Language Process (다국어 통합 프로세스)</t>
+          <t xml:space="preserve">   목적: 지능적인 로직을 사용하여 이전 작업을 새 베이스라인에 가져오기</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr"/>
@@ -777,7 +780,7 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   목적: 세 가지 언어 버전(한국어/영어/중국어)을 하나의 파일로 병합 및 업데이트</t>
+          <t xml:space="preserve">   사용 시점: 완료된 번역을 보존하는 작업 파일 준비가 필요할 때</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr"/>
@@ -786,30 +789,30 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   사용 시점: 유연한 업데이트가 필요한 다국어 프로젝트 관리 시</t>
+          <t xml:space="preserve">   출력물: 번역 작업이 가능한 Work Transform 파일</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr"/>
       <c r="C24" s="2" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   출력물: 선택적 언어 업데이트가 적용된 통합 다국어 파일</t>
-        </is>
-      </c>
+      <c r="A25" s="2" t="inlineStr"/>
       <c r="B25" s="2" t="inlineStr"/>
       <c r="C25" s="2" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr"/>
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>3. All Language Process (다국어 통합 프로세스)</t>
+        </is>
+      </c>
       <c r="B26" s="2" t="inlineStr"/>
       <c r="C26" s="2" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>4. Master File Update (마스터 파일 업데이트)</t>
+          <t xml:space="preserve">   목적: 세 가지 언어 버전(한국어/영어/중국어)을 하나의 파일로 병합 및 업데이트</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr"/>
@@ -818,7 +821,7 @@
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   목적: Working Process의 완료된 작업을 마스터 파일에 동기화</t>
+          <t xml:space="preserve">   사용 시점: 유연한 업데이트가 필요한 다국어 프로젝트 관리 시</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr"/>
@@ -827,60 +830,62 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   사용 시점: 번역 완료 후 공식 마스터 파일 업데이트가 필요할 때</t>
+          <t xml:space="preserve">   출력물: 선택적 언어 업데이트가 적용된 통합 다국어 파일</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr"/>
       <c r="C29" s="2" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   출력물: High/Low 중요도로 분리된 업데이트된 마스터 파일</t>
-        </is>
-      </c>
+      <c r="A30" s="2" t="inlineStr"/>
       <c r="B30" s="2" t="inlineStr"/>
       <c r="C30" s="2" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr"/>
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>4. Master File Update (마스터 파일 업데이트)</t>
+        </is>
+      </c>
       <c r="B31" s="2" t="inlineStr"/>
       <c r="C31" s="2" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>주요 기능</t>
+          <t xml:space="preserve">   목적: Working Process의 완료된 작업을 마스터 파일에 동기화</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr"/>
       <c r="C32" s="2" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr"/>
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   사용 시점: 번역 완료 후 공식 마스터 파일 업데이트가 필요할 때</t>
+        </is>
+      </c>
       <c r="B33" s="2" t="inlineStr"/>
       <c r="C33" s="2" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>✓ 10-Key 패턴 매칭 + TWO-PASS 알고리즘</t>
+          <t xml:space="preserve">   출력물: High/Low 중요도로 분리된 업데이트된 마스터 파일</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr"/>
       <c r="C34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  포괄적인 10-key 조합 (3-key + 2-key)과 TWO-PASS로 1-to-many 매칭 방지</t>
-        </is>
-      </c>
+      <c r="A35" s="2" t="inlineStr"/>
+      <c r="B35" s="2" t="inlineStr"/>
+      <c r="C35" s="2" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  EventName과 StrOrigin을 모두 룩업 키로 사용하여 EventName 변경 자동 처리</t>
+          <t>주요 기능</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr"/>
@@ -894,176 +899,184 @@
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>✓ 지능적인 Import 로직</t>
+          <t>✓ 10-Key 패턴 매칭 + TWO-PASS 알고리즘</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr"/>
       <c r="C38" s="2" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  녹음 STATUS를 분석하여 번역 데이터 보존 또는 업데이트 여부 자동 결정</t>
-        </is>
-      </c>
-      <c r="B39" s="2" t="inlineStr"/>
-      <c r="C39" s="2" t="inlineStr"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  포괄적인 10-key 조합 (3-key + 2-key)과 TWO-PASS로 1-to-many 매칭 방지</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="inlineStr"/>
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  EventName과 StrOrigin을 모두 룩업 키로 사용하여 EventName 변경 자동 처리</t>
+        </is>
+      </c>
       <c r="B40" s="2" t="inlineStr"/>
       <c r="C40" s="2" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="inlineStr">
-        <is>
-          <t>✓ 유연한 다국어 지원</t>
-        </is>
-      </c>
+      <c r="A41" s="2" t="inlineStr"/>
       <c r="B41" s="2" t="inlineStr"/>
       <c r="C41" s="2" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  필요한 언어만 업데이트하고 나머지는 자동으로 보존</t>
+          <t>✓ 지능적인 Import 로직</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr"/>
       <c r="C42" s="2" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr"/>
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  녹음 STATUS를 분석하여 번역 데이터 보존 또는 업데이트 여부 자동 결정</t>
+        </is>
+      </c>
       <c r="B43" s="2" t="inlineStr"/>
       <c r="C43" s="2" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="inlineStr">
-        <is>
-          <t>✓ 완벽한 업데이트 히스토리</t>
-        </is>
-      </c>
+      <c r="A44" s="2" t="inlineStr"/>
       <c r="B44" s="2" t="inlineStr"/>
       <c r="C44" s="2" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  모든 프로세스 실행이 상세한 통계 및 파일 정보와 함께 기록됨</t>
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>✓ 유연한 다국어 지원</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr"/>
       <c r="C45" s="2" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="inlineStr"/>
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  필요한 언어만 업데이트하고 나머지는 자동으로 보존</t>
+        </is>
+      </c>
       <c r="B46" s="2" t="inlineStr"/>
       <c r="C46" s="2" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="inlineStr">
-        <is>
-          <t>✓ 시각적 변경 분류</t>
-        </is>
-      </c>
+      <c r="A47" s="2" t="inlineStr"/>
       <c r="B47" s="2" t="inlineStr"/>
       <c r="C47" s="2" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  색상 코딩된 변경 유형으로 주의가 필요한 항목을 쉽게 식별</t>
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>✓ 완벽한 업데이트 히스토리</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr"/>
       <c r="C48" s="2" t="inlineStr"/>
     </row>
-    <row r="49"/>
-    <row r="50"/>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  모든 프로세스 실행이 상세한 통계 및 파일 정보와 함께 기록됨</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr"/>
+      <c r="C49" s="2" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr"/>
+      <c r="B50" s="2" t="inlineStr"/>
+      <c r="C50" s="2" t="inlineStr"/>
+    </row>
     <row r="51">
-      <c r="A51" s="13" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>✓ 시각적 변경 분류</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr"/>
+      <c r="C51" s="2" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  색상 코딩된 변경 유형으로 주의가 필요한 항목을 쉽게 식별</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr"/>
+      <c r="C52" s="2" t="inlineStr"/>
+    </row>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" s="13" t="inlineStr">
         <is>
           <t>v1116의 새로운 기능 (TWO-PASS 알고리즘)</t>
         </is>
       </c>
     </row>
-    <row r="52"/>
-    <row r="53">
-      <c r="A53" s="9" t="inlineStr">
+    <row r="56"/>
+    <row r="57">
+      <c r="A57" s="9" t="inlineStr">
         <is>
           <t>✅ TWO-PASS 알고리즘</t>
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="58">
+      <c r="A58" t="inlineStr">
         <is>
           <t xml:space="preserve">  - PASS 1: 확실한 항목 감지 및 마킹 (변경 없음, 신규, 삭제)</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - PASS 2: 마크되지 않은 행만 사용한 패턴 매칭</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - 1-to-many 매칭 문제 제거</t>
-        </is>
-      </c>
-    </row>
-    <row r="57"/>
-    <row r="58">
-      <c r="A58" s="9" t="inlineStr">
-        <is>
-          <t>✅ 100% 정확한 중복 처리</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 중복 StrOrigin 처리 (예: "안녕하세요", "예", "아니오")</t>
+          <t xml:space="preserve">  - PASS 2: 마크되지 않은 행만 사용한 패턴 매칭</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 빈 StrOrigin 처리 (빈 셀)</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - 중복 CastingKey 처리 (동일한 캐릭터가 여러 번 말하는 경우)</t>
-        </is>
-      </c>
-    </row>
-    <row r="62"/>
+          <t xml:space="preserve">  - 1-to-many 매칭 문제 제거</t>
+        </is>
+      </c>
+    </row>
+    <row r="61"/>
+    <row r="62">
+      <c r="A62" s="9" t="inlineStr">
+        <is>
+          <t>✅ 100% 정확한 중복 처리</t>
+        </is>
+      </c>
+    </row>
     <row r="63">
-      <c r="A63" s="9" t="inlineStr">
-        <is>
-          <t>✅ 수학적으로 정확한 행 계산</t>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - 중복 StrOrigin 처리 (예: "안녕하세요", "예", "아니오")</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 공식: new_rows - deleted_rows = actual_difference</t>
+          <t xml:space="preserve">  - 빈 StrOrigin 처리 (빈 셀)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 항상 정확, 불일치 없음</t>
+          <t xml:space="preserve">  - 중복 CastingKey 처리 (동일한 캐릭터가 여러 번 말하는 경우)</t>
         </is>
       </c>
     </row>
@@ -1071,122 +1084,122 @@
     <row r="67">
       <c r="A67" s="9" t="inlineStr">
         <is>
-          <t>✅ 동일한 감지 로직</t>
+          <t>✅ 수학적으로 정확한 행 계산</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 모든 4개 프로세서 (Raw, Working, All Language, Master)가 동일한 알고리즘 사용</t>
+          <t xml:space="preserve">  - 공식: new_rows - deleted_rows = actual_difference</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 모든 프로세스에서 일관된 결과</t>
+          <t xml:space="preserve">  - 항상 정확, 불일치 없음</t>
         </is>
       </c>
     </row>
     <row r="70"/>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>✅ 전체 중복 행 정리</t>
+      <c r="A71" s="9" t="inlineStr">
+        <is>
+          <t>✅ 동일한 감지 로직</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - 처리 전 전체 중복 행 자동 제거</t>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - 모든 4개 프로세서 (Raw, Working, All Language, Master)가 동일한 알고리즘 사용</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 분석을 위한 깨끗한 데이터 보장</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="9" t="inlineStr">
-        <is>
-          <t>✅ TWO-PASS 알고리즘 - 1-to-many 매칭 문제 제거</t>
-        </is>
-      </c>
-    </row>
+          <t xml:space="preserve">  - 모든 프로세스에서 일관된 결과</t>
+        </is>
+      </c>
+    </row>
+    <row r="74"/>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • PASS 1: 확실한 항목 감지 및 마킹 (변경 없음, 신규, 삭제)</t>
+          <t>✅ 전체 중복 행 정리</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • PASS 2: 마크되지 않은 행만 사용한 패턴 매칭</t>
+      <c r="A76" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - 처리 전 전체 중복 행 자동 제거</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 각 PREVIOUS 행이 최대 한 개의 CURRENT 행과만 매칭되도록 보장</t>
-        </is>
-      </c>
-    </row>
-    <row r="78"/>
+          <t xml:space="preserve">  - 분석을 위한 깨끗한 데이터 보장</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="9" t="inlineStr">
+        <is>
+          <t>✅ TWO-PASS 알고리즘 - 1-to-many 매칭 문제 제거</t>
+        </is>
+      </c>
+    </row>
     <row r="79">
-      <c r="A79" s="9" t="inlineStr">
-        <is>
-          <t>✅ 100% 정확한 중복 처리</t>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • PASS 1: 확실한 항목 감지 및 마킹 (변경 없음, 신규, 삭제)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 중복 StrOrigin 처리 (예: "안녕하세요", "예", "아니오")</t>
+          <t xml:space="preserve">  • PASS 2: 마크되지 않은 행만 사용한 패턴 매칭</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 빈 StrOrigin 처리 (빈 셀)</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 중복 CastingKey 처리 (동일한 캐릭터가 여러 번 말하는 경우)</t>
-        </is>
-      </c>
-    </row>
-    <row r="83"/>
+          <t xml:space="preserve">  • 각 PREVIOUS 행이 최대 한 개의 CURRENT 행과만 매칭되도록 보장</t>
+        </is>
+      </c>
+    </row>
+    <row r="82"/>
+    <row r="83">
+      <c r="A83" s="9" t="inlineStr">
+        <is>
+          <t>✅ 100% 정확한 중복 처리</t>
+        </is>
+      </c>
+    </row>
     <row r="84">
-      <c r="A84" s="9" t="inlineStr">
-        <is>
-          <t>✅ 수학적으로 정확한 행 계산</t>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 중복 StrOrigin 처리 (예: "안녕하세요", "예", "아니오")</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 공식: new_rows - deleted_rows = actual_difference</t>
+          <t xml:space="preserve">  • 빈 StrOrigin 처리 (빈 셀)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 항상 정확, 불일치 없음</t>
+          <t xml:space="preserve">  • 중복 CastingKey 처리 (동일한 캐릭터가 여러 번 말하는 경우)</t>
         </is>
       </c>
     </row>
@@ -1194,81 +1207,81 @@
     <row r="88">
       <c r="A88" s="9" t="inlineStr">
         <is>
-          <t>✅ 모든 4개 프로세서에서 동일한 감지 로직</t>
+          <t>✅ 수학적으로 정확한 행 계산</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • Raw, Working, All Language, Master 프로세서 모두 동일한 알고리즘 사용</t>
+          <t xml:space="preserve">  • 공식: new_rows - deleted_rows = actual_difference</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 항상 정확, 불일치 없음</t>
+        </is>
+      </c>
+    </row>
+    <row r="91"/>
+    <row r="92">
+      <c r="A92" s="9" t="inlineStr">
+        <is>
+          <t>✅ 모든 4개 프로세서에서 동일한 감지 로직</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Raw, Working, All Language, Master 프로세서 모두 동일한 알고리즘 사용</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • 모든 프로세스에서 일관된 결과</t>
         </is>
       </c>
     </row>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93">
-      <c r="A93" s="8" t="inlineStr">
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97">
+      <c r="A97" s="8" t="inlineStr">
         <is>
           <t>v1117의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="94"/>
-    <row r="95">
-      <c r="A95" s="9" t="inlineStr">
+    <row r="98"/>
+    <row r="99">
+      <c r="A99" s="9" t="inlineStr">
         <is>
           <t>✅ Master File Update - TimeFrame 보존 로직 (High Importance만 해당)</t>
         </is>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
+    <row r="100">
+      <c r="A100" t="inlineStr">
         <is>
           <t xml:space="preserve">  • TimeFrame 변경 AND StrOrigin 변경 → TimeFrame 업데이트 (SOURCE 사용)</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 모든 변경 조합에 대해 작동 (강력하고 범용적)</t>
-        </is>
-      </c>
-    </row>
-    <row r="99"/>
-    <row r="100">
-      <c r="A100" s="9" t="inlineStr">
-        <is>
-          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame 업데이트는 대사 내용 변경과 함께 발생할 때만 적용</t>
+          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 대사 내용은 동일하지만 타이밍만 변경된 경우 원치 않는 업데이트 방지</t>
+          <t xml:space="preserve">  • 모든 변경 조합에 대해 작동 (강력하고 범용적)</t>
         </is>
       </c>
     </row>
@@ -1276,828 +1289,850 @@
     <row r="104">
       <c r="A104" s="9" t="inlineStr">
         <is>
-          <t>예시:</t>
+          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1. TimeFrame + StrOrigin 둘 다 변경 → TimeFrame 업데이트 ✅</t>
+          <t xml:space="preserve">  • TimeFrame 업데이트는 대사 내용 변경과 함께 발생할 때만 적용</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 대사 내용은 동일하지만 타이밍만 변경된 경우 원치 않는 업데이트 방지</t>
+        </is>
+      </c>
+    </row>
+    <row r="107"/>
+    <row r="108">
+      <c r="A108" s="9" t="inlineStr">
+        <is>
+          <t>예시:</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. TimeFrame + StrOrigin 둘 다 변경 → TimeFrame 업데이트 ✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
           <t xml:space="preserve">  2. TimeFrame + StrOrigin + EventName 모두 변경 → TimeFrame 업데이트 ✅</t>
         </is>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
+    <row r="111">
+      <c r="A111" t="inlineStr">
         <is>
           <t xml:space="preserve">  3. TimeFrame만 변경 (StrOrigin 동일) → TimeFrame 보존 (TARGET 유지) ✅</t>
         </is>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
+    <row r="112">
+      <c r="A112" t="inlineStr">
         <is>
           <t xml:space="preserve">  4. TimeFrame + EventName 변경 (StrOrigin 동일) → TimeFrame 보존 (TARGET 유지) ✅</t>
         </is>
       </c>
     </row>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111">
-      <c r="A111" s="8" t="inlineStr">
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115">
+      <c r="A115" s="8" t="inlineStr">
         <is>
           <t>v1117의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="112"/>
-    <row r="113">
-      <c r="A113" s="9" t="inlineStr">
-        <is>
-          <t>✅ Master File Update - TimeFrame 보존 로직 (High Importance만 해당)</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • TimeFrame 변경 AND StrOrigin 변경 → TimeFrame 업데이트 (SOURCE 사용)</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 모든 변경 조합에 대해 작동 (강력하고 범용적)</t>
-        </is>
-      </c>
-    </row>
+    <row r="116"/>
     <row r="117">
       <c r="A117" s="9" t="inlineStr">
         <is>
-          <t>중요한 이유:</t>
+          <t>✅ Master File Update - TimeFrame 보존 로직 (High Importance만 해당)</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame 업데이트는 대사 내용 변경과 함께 발생할 때만 적용</t>
+          <t xml:space="preserve">  • TimeFrame 변경 AND StrOrigin 변경 → TimeFrame 업데이트 (SOURCE 사용)</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 대사 내용은 동일하지만 타이밍만 변경된 경우 원치 않는 업데이트 방지</t>
+          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="9" t="inlineStr">
-        <is>
-          <t>예시:</t>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 모든 변경 조합에 대해 작동 (강력하고 범용적)</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 1. TimeFrame + StrOrigin 둘 다 변경 → TimeFrame 업데이트 ✅</t>
+      <c r="A121" s="9" t="inlineStr">
+        <is>
+          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 2. TimeFrame + StrOrigin + EventName 모두 변경 → TimeFrame 업데이트 ✅</t>
+          <t xml:space="preserve">  • TimeFrame 업데이트는 대사 내용 변경과 함께 발생할 때만 적용</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 대사 내용은 동일하지만 타이밍만 변경된 경우 원치 않는 업데이트 방지</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="9" t="inlineStr">
+        <is>
+          <t>예시:</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 1. TimeFrame + StrOrigin 둘 다 변경 → TimeFrame 업데이트 ✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 2. TimeFrame + StrOrigin + EventName 모두 변경 → TimeFrame 업데이트 ✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • 3. TimeFrame만 변경 (StrOrigin 동일) → TimeFrame 보존 (TARGET 유지) ✅</t>
         </is>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
+    <row r="128">
+      <c r="A128" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 4. TimeFrame + EventName 변경 (StrOrigin 동일) → TimeFrame 보존 (TARGET 유지) ✅</t>
         </is>
       </c>
     </row>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127">
-      <c r="A127" s="8" t="inlineStr">
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131">
+      <c r="A131" s="8" t="inlineStr">
         <is>
           <t>v1117.1의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="128"/>
-    <row r="129">
-      <c r="A129" s="9" t="inlineStr">
+    <row r="132"/>
+    <row r="133">
+      <c r="A133" s="9" t="inlineStr">
         <is>
           <t>✅ 컬럼 견고성 수정 (모든 프로세스)</t>
         </is>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
+    <row r="134">
+      <c r="A134" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 서로 다른 컬럼 구조를 가진 파일을 우아하게 처리</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 두 파일(PREVIOUS와 CURRENT)에 모두 존재하는 컬럼만 비교</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 선택적 컬럼이 없어도 충돌 없음 (Desc, StartFrame, EndFrame, Text 등)</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 필수 핵심 컬럼: SequenceName, EventName, StrOrigin, CastingKey 구성요소</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="9" t="inlineStr">
-        <is>
-          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 이전 파일은 최신 파일보다 컬럼 수가 적을 수 있음</t>
+          <t xml:space="preserve">  • 두 파일(PREVIOUS와 CURRENT)에 모두 존재하는 컬럼만 비교</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 핵심 키만 있으면 프로그램이 완벽하게 실행됨</t>
+          <t xml:space="preserve">  • 선택적 컬럼이 없어도 충돌 없음 (Desc, StartFrame, EndFrame, Text 등)</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 없는 선택적 컬럼에 대한 변경 감지를 우아하게 건너뜀</t>
+          <t xml:space="preserve">  • 필수 핵심 컬럼: SequenceName, EventName, StrOrigin, CastingKey 구성요소</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="9" t="inlineStr">
         <is>
-          <t>✅ v1117 - Master File Update - TimeFrame 보존 로직 (High Importance만 해당)</t>
+          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame 변경 AND StrOrigin 변경 → TimeFrame 업데이트 (SOURCE 사용)</t>
+          <t xml:space="preserve">  • 이전 파일은 최신 파일보다 컬럼 수가 적을 수 있음</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
+          <t xml:space="preserve">  • 핵심 키만 있으면 프로그램이 완벽하게 실행됨</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 없는 선택적 컬럼에 대한 변경 감지를 우아하게 건너뜀</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1117 - Master File Update - TimeFrame 보존 로직 (High Importance만 해당)</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame 변경 AND StrOrigin 변경 → TimeFrame 업데이트 (SOURCE 사용)</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame 변경 BUT StrOrigin 변경 안 됨 → TimeFrame 보존 (TARGET 유지)</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • 모든 변경 조합에 대해 작동 (강력하고 범용적)</t>
         </is>
       </c>
     </row>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144">
-      <c r="A144" s="8" t="inlineStr">
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148">
+      <c r="A148" s="8" t="inlineStr">
         <is>
           <t>v1118.3의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="145"/>
-    <row r="146">
-      <c r="A146" s="9" t="inlineStr">
+    <row r="149"/>
+    <row r="150">
+      <c r="A150" s="9" t="inlineStr">
         <is>
           <t>✅ Master File Update - TimeFrame 보존 복원 (v1118.3)</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • StartFrame 변경 BUT StrOrigin 변경 안 됨 → StartFrame 보존 (TARGET 유지)</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 대사 내용이 변경되지 않았을 때 원치 않는 타이밍 업데이트 방지</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TARGET에서 EventName 매치가 있는 HIGH importance 행에 적용</t>
+          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
         </is>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="9" t="inlineStr">
-        <is>
-          <t>중요한 이유:</t>
+      <c r="A152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • StartFrame은 대사 내용도 변경될 때만 업데이트되어야 함</t>
+          <t xml:space="preserve">  • StartFrame 변경 BUT StrOrigin 변경 안 됨 → StartFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 타이밍만 변경되고 대사는 동일한 경우 기존 StartFrame 유지</t>
+          <t xml:space="preserve">  • 대사 내용이 변경되지 않았을 때 원치 않는 타이밍 업데이트 방지</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • v1117에 있던 기능이 v1118.2 간소화 시 제거되었으나 이제 복원됨</t>
+          <t xml:space="preserve">  • TARGET에서 EventName 매치가 있는 HIGH importance 행에 적용</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="9" t="inlineStr">
         <is>
-          <t>✅ v1118.2 - 간소화된 Master File Update 로직</t>
+          <t>중요한 이유:</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • EventName만으로 매칭 (Master File Update에는 10-key 시스템 미사용)</t>
+          <t xml:space="preserve">  • StartFrame은 대사 내용도 변경될 때만 업데이트되어야 함</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • CHANGES 컬럼은 항상 SOURCE에서 보존됨 (재계산하지 않음)</t>
+          <t xml:space="preserve">  • 타이밍만 변경되고 대사는 동일한 경우 기존 StartFrame 유지</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • LOW importance 행은 완전히 건너뜀 (처리하지 않음)</t>
+          <t xml:space="preserve">  • v1117에 있던 기능이 v1118.2 간소화 시 제거되었으나 이제 복원됨</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 단일 출력 시트 (HIGH + DELETED 행 결합)</t>
+      <c r="A160" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.2 - 간소화된 Master File Update 로직</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • EventName만으로 매칭 (Master File Update에는 10-key 시스템 미사용)</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES 컬럼은 항상 SOURCE에서 보존됨 (재계산하지 않음)</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • LOW importance 행은 완전히 건너뜀 (처리하지 않음)</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 단일 출력 시트 (HIGH + DELETED 행 결합)</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • 간단한 데이터 이동 작업 (비교 작업 아님)</t>
         </is>
       </c>
     </row>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164">
-      <c r="A164" s="8" t="inlineStr">
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168">
+      <c r="A168" s="8" t="inlineStr">
         <is>
           <t>v1118.4의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="165"/>
-    <row r="166">
-      <c r="A166" s="9" t="inlineStr">
+    <row r="169"/>
+    <row r="170">
+      <c r="A170" s="9" t="inlineStr">
         <is>
           <t>✅ 향상된 슈퍼 그룹 단어 분석 (v1118.4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 새로운 기능: 'Other' 슈퍼 그룹 - 포함: Police, Minigame, Trade, Church, Shop, Contribution, RoyalSupply, Research, Quest Groups, faction_etc</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 이름 변경: 포괄적인 'Other' → 'Everything Else' (더 명확한 의미)</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 새로운 기능: Translation % (Previous) - 이전 버전의 번역 진행 상황 추적</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 새로운 기능: Translation % Change - 번역 진행률 차이 확인</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words' → 'Untranslated Words (Remaining to Translate)'</t>
+          <t xml:space="preserve">  • 새로운 기능: 'Other' 슈퍼 그룹 - 포함: Police, Minigame, Trade, Church, Shop, Contribution, RoyalSupply, Research, Quest Groups, faction_etc</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 컬럼 재구성: 가장 중요한 지표를 먼저 배치, 관련 데이터를 그룹화</t>
+          <t xml:space="preserve">  • 이름 변경: 포괄적인 'Other' → 'Everything Else' (더 명확한 의미)</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 'Everything Else'를 설명하는 참고 사항을 표 아래에 추가</t>
+          <t xml:space="preserve">  • 새로운 기능: Translation % (Previous) - 이전 버전의 번역 진행 상황 추적</t>
         </is>
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="9" t="inlineStr">
-        <is>
-          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
+      <c r="A174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 새로운 기능: Translation % Change - 번역 진행률 차이 확인</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
+          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words' → 'Untranslated Words (Remaining to Translate)'</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
+          <t xml:space="preserve">  • 컬럼 재구성: 가장 중요한 지표를 먼저 배치, 관련 데이터를 그룹화</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+          <t xml:space="preserve">  • 'Everything Else'를 설명하는 참고 사항을 표 아래에 추가</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="9" t="inlineStr">
         <is>
-          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • StartFrame 변경 BUT StrOrigin 변경 안 됨 → StartFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
+    <row r="186">
+      <c r="A186" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 대사 내용이 변경되지 않았을 때 원치 않는 타이밍 업데이트 방지</t>
         </is>
       </c>
     </row>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185">
-      <c r="A185" s="8" t="inlineStr">
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189">
+      <c r="A189" s="8" t="inlineStr">
         <is>
           <t>v1118.6의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="186"/>
-    <row r="187">
-      <c r="A187" s="9" t="inlineStr">
+    <row r="190"/>
+    <row r="191">
+      <c r="A191" s="9" t="inlineStr">
         <is>
           <t>✅ 중요 버그 수정 (v1118.6)</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: Working VRS Check에서 TypeError 'unhashable type: dict' 오류</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: 모든 DataFrame 컬럼 접근이 safe_str() 패턴 사용</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: 룩업 사전이 이제 인덱스를 올바르게 저장 (dict 객체 아님)</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 테스트 완료: 5000행 포괄적 테스트로 100% 정확도 검증</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 테스트 완료: 모든 프로세서 (Raw, Working, All Language)가 실제 데이터로 통과</t>
+          <t xml:space="preserve">  • 수정됨: Working VRS Check에서 TypeError 'unhashable type: dict' 오류</t>
         </is>
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="9" t="inlineStr">
-        <is>
-          <t>✅ 향상된 슈퍼 그룹 단어 분석 (v1118.4)</t>
+      <c r="A193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 수정됨: 모든 DataFrame 컬럼 접근이 safe_str() 패턴 사용</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 새로운 기능: 'Other' 슈퍼 그룹 - 포함: Police, Minigame, Trade, Church, Shop, Contribution, RoyalSupply, Research, Quest Groups, faction_etc</t>
+          <t xml:space="preserve">  • 수정됨: 룩업 사전이 이제 인덱스를 올바르게 저장 (dict 객체 아님)</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 이름 변경: 포괄적인 'Other' → 'Everything Else' (더 명확한 의미)</t>
+          <t xml:space="preserve">  • 테스트 완료: 5000행 포괄적 테스트로 100% 정확도 검증</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 새로운 기능: Translation % (Previous) - 이전 버전의 번역 진행 상황 추적</t>
+          <t xml:space="preserve">  • 테스트 완료: 모든 프로세서 (Raw, Working, All Language)가 실제 데이터로 통과</t>
         </is>
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 새로운 기능: Translation % Change - 번역 진행률 차이 확인</t>
+      <c r="A197" s="9" t="inlineStr">
+        <is>
+          <t>✅ 향상된 슈퍼 그룹 단어 분석 (v1118.4)</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words' → 'Untranslated Words (Remaining to Translate)'</t>
+          <t xml:space="preserve">  • 새로운 기능: 'Other' 슈퍼 그룹 - 포함: Police, Minigame, Trade, Church, Shop, Contribution, RoyalSupply, Research, Quest Groups, faction_etc</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 컬럼 재구성: 가장 중요한 지표를 먼저 배치, 관련 데이터를 그룹화</t>
+          <t xml:space="preserve">  • 이름 변경: 포괄적인 'Other' → 'Everything Else' (더 명확한 의미)</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 'Everything Else'를 설명하는 참고 사항을 표 아래에 추가</t>
+          <t xml:space="preserve">  • 새로운 기능: Translation % (Previous) - 이전 버전의 번역 진행 상황 추적</t>
         </is>
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="9" t="inlineStr">
-        <is>
-          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
+      <c r="A201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 새로운 기능: Translation % Change - 번역 진행률 차이 확인</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
+          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words' → 'Untranslated Words (Remaining to Translate)'</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
+          <t xml:space="preserve">  • 컬럼 재구성: 가장 중요한 지표를 먼저 배치, 관련 데이터를 그룹화</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+          <t xml:space="preserve">  • 'Everything Else'를 설명하는 참고 사항을 표 아래에 추가</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="9" t="inlineStr">
         <is>
-          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • StartFrame 변경 BUT StrOrigin 변경 안 됨 → StartFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
+    <row r="213">
+      <c r="A213" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 대사 내용이 변경되지 않았을 때 원치 않는 타이밍 업데이트 방지</t>
         </is>
       </c>
     </row>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212">
-      <c r="A212" s="8" t="inlineStr">
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216">
+      <c r="A216" s="8" t="inlineStr">
         <is>
           <t>v1118.6의 새로운 기능</t>
         </is>
       </c>
     </row>
-    <row r="213"/>
-    <row r="214">
-      <c r="A214" s="9" t="inlineStr">
+    <row r="217"/>
+    <row r="218">
+      <c r="A218" s="9" t="inlineStr">
         <is>
           <t>✅ 중요 버그 수정 (v1118.6)</t>
-        </is>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: Working VRS Check에서 TypeError 'unhashable type: dict' 오류</t>
-        </is>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: 모든 DataFrame 컬럼 접근이 safe_str() 패턴 사용</t>
-        </is>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 수정됨: 룩업 사전이 이제 인덱스를 올바르게 저장 (dict 객체 아님)</t>
-        </is>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 테스트 완료: 5000행 포괄적 테스트로 100% 정확도 검증</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 테스트 완료: 모든 프로세서 (Raw, Working, All Language)가 실제 데이터로 통과</t>
+          <t xml:space="preserve">  • 수정됨: Working VRS Check에서 TypeError 'unhashable type: dict' 오류</t>
         </is>
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="9" t="inlineStr">
-        <is>
-          <t>✅ Phase 2.2.1 완료 - 슈퍼 그룹 분석 개선 (v1118.4)</t>
+      <c r="A220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 수정됨: 모든 DataFrame 컬럼 접근이 safe_str() 패턴 사용</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 제거됨: 'Others' 슈퍼 그룹 및 stageclosedialog 체크 완전히 제거</t>
+          <t xml:space="preserve">  • 수정됨: 룩업 사전이 이제 인덱스를 올바르게 저장 (dict 객체 아님)</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 재정렬: 슈퍼 그룹 - AI Dialog가 이제 Quest Dialog 앞에 표시됨</t>
+          <t xml:space="preserve">  • 테스트 완료: 5000행 포괄적 테스트로 100% 정확도 검증</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words (Remaining to Translate)' → 'Not Translated'</t>
+          <t xml:space="preserve">  • 테스트 완료: 모든 프로세서 (Raw, Working, All Language)가 실제 데이터로 통과</t>
         </is>
       </c>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 제거됨: 메인 테이블에서 마이그레이션 컬럼 제거 (Words Migrated In/Out)</t>
+      <c r="A224" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 2.2.1 완료 - 슈퍼 그룹 분석 개선 (v1118.4)</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 추가됨: 메인 테이블 아래에 상세한 'Super Group Migrations' 테이블</t>
+          <t xml:space="preserve">  • 제거됨: 'Others' 슈퍼 그룹 및 stageclosedialog 체크 완전히 제거</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 모든 마이그레이션에 대한 소스 → 목적지 쌍과 단어 수 표시</t>
+          <t xml:space="preserve">  • 재정렬: 슈퍼 그룹 - AI Dialog가 이제 Quest Dialog 앞에 표시됨</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 업데이트: 테이블 아래 설명 노트 ('Others' 참조 제거)</t>
+          <t xml:space="preserve">  • 이름 변경: 'Untranslated Words (Remaining to Translate)' → 'Not Translated'</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 총 8개의 슈퍼 그룹: Main Chapters, F1, F2, F3, AI Dialog, Quest Dialog, Other, Everything Else</t>
+          <t xml:space="preserve">  • 제거됨: 메인 테이블에서 마이그레이션 컬럼 제거 (Words Migrated In/Out)</t>
         </is>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="9" t="inlineStr">
-        <is>
-          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
+      <c r="A229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 추가됨: 메인 테이블 아래에 상세한 'Super Group Migrations' 테이블</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
+          <t xml:space="preserve">  • 모든 마이그레이션에 대한 소스 → 목적지 쌍과 단어 수 표시</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
+          <t xml:space="preserve">  • 업데이트: 테이블 아래 설명 노트 ('Others' 참조 제거)</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+          <t xml:space="preserve">  • 총 8개의 슈퍼 그룹: Main Chapters, F1, F2, F3, AI Dialog, Quest Dialog, Other, Everything Else</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="9" t="inlineStr">
         <is>
-          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+          <t>컬럼 순서 (가독성 향상을 위해 재구성):</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+          <t xml:space="preserve">  • 1. 슈퍼 그룹 이름, 총 단어 수 (현재/이전), 순 변화, % 변화</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+          <t xml:space="preserve">  • 2. 번역/미번역 단어, 번역 % (현재/이전/변화)</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
+          <t xml:space="preserve">  • 3. 상세 분석: 추가/삭제/변경/미변경/마이그레이션된 단어</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame 보존 복원</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame만 해당 (EndFrame은 항상 SOURCE에서 업데이트)</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • StartFrame 변경 AND StrOrigin 변경 → StartFrame 업데이트 (SOURCE 사용)</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • StartFrame 변경 BUT StrOrigin 변경 안 됨 → StartFrame 보존 (TARGET 유지)</t>
         </is>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" t="inlineStr">
+    <row r="241">
+      <c r="A241" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 대사 내용이 변경되지 않았을 때 원치 않는 타이밍 업데이트 방지</t>
         </is>
@@ -2268,7 +2303,6 @@
         </is>
       </c>
     </row>
-    <row r="20"/>
     <row r="21">
       <c r="A21" s="17" t="inlineStr">
         <is>
@@ -2313,7 +2347,6 @@
         </is>
       </c>
     </row>
-    <row r="27"/>
     <row r="28">
       <c r="A28" s="21" t="inlineStr">
         <is>
@@ -2321,7 +2354,6 @@
         </is>
       </c>
     </row>
-    <row r="29"/>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
@@ -2499,7 +2531,6 @@
       <c r="B50" s="2" t="inlineStr"/>
       <c r="C50" s="2" t="inlineStr"/>
     </row>
-    <row r="51"/>
     <row r="52">
       <c r="A52" s="9" t="inlineStr">
         <is>
@@ -2507,7 +2538,6 @@
         </is>
       </c>
     </row>
-    <row r="53"/>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
@@ -2522,7 +2552,6 @@
         </is>
       </c>
     </row>
-    <row r="56"/>
     <row r="57">
       <c r="A57" s="19" t="inlineStr">
         <is>
@@ -2537,7 +2566,6 @@
         </is>
       </c>
     </row>
-    <row r="59"/>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
@@ -2566,7 +2594,6 @@
         </is>
       </c>
     </row>
-    <row r="64"/>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
@@ -2588,7 +2615,6 @@
         </is>
       </c>
     </row>
-    <row r="68"/>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
@@ -2603,7 +2629,6 @@
         </is>
       </c>
     </row>
-    <row r="71"/>
     <row r="72">
       <c r="A72" s="20" t="inlineStr">
         <is>
@@ -2618,7 +2643,6 @@
         </is>
       </c>
     </row>
-    <row r="74"/>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
@@ -2661,7 +2685,6 @@
         </is>
       </c>
     </row>
-    <row r="81"/>
     <row r="82">
       <c r="A82" s="21" t="inlineStr">
         <is>
@@ -2669,7 +2692,6 @@
         </is>
       </c>
     </row>
-    <row r="83"/>
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
@@ -3079,7 +3101,6 @@
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr"/>
     </row>
-    <row r="13"/>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -4220,7 +4241,6 @@
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr"/>
     </row>
-    <row r="12"/>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
@@ -5365,7 +5385,6 @@
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr"/>
     </row>
-    <row r="12"/>
     <row r="13">
       <c r="A13" s="21" t="inlineStr">
         <is>
@@ -5373,7 +5392,6 @@
         </is>
       </c>
     </row>
-    <row r="14"/>
     <row r="15">
       <c r="A15" s="23" t="inlineStr">
         <is>
@@ -5402,7 +5420,6 @@
         </is>
       </c>
     </row>
-    <row r="19"/>
     <row r="20">
       <c r="A20" s="24" t="inlineStr">
         <is>
@@ -5438,7 +5455,6 @@
         </is>
       </c>
     </row>
-    <row r="25"/>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
@@ -5512,7 +5528,6 @@
       <c r="B34" s="2" t="inlineStr"/>
       <c r="C34" s="2" t="inlineStr"/>
     </row>
-    <row r="35"/>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
@@ -6591,8 +6606,6 @@
       <c r="B167" s="2" t="inlineStr"/>
       <c r="C167" s="2" t="inlineStr"/>
     </row>
-    <row r="168"/>
-    <row r="169"/>
     <row r="170">
       <c r="A170" s="25" t="inlineStr">
         <is>
@@ -6600,7 +6613,6 @@
         </is>
       </c>
     </row>
-    <row r="171"/>
     <row r="172">
       <c r="A172" s="9" t="inlineStr">
         <is>
@@ -6622,7 +6634,6 @@
         </is>
       </c>
     </row>
-    <row r="175"/>
     <row r="176">
       <c r="A176" s="26" t="inlineStr">
         <is>
@@ -6630,8 +6641,6 @@
         </is>
       </c>
     </row>
-    <row r="177"/>
-    <row r="178"/>
     <row r="179">
       <c r="A179" s="25" t="inlineStr">
         <is>
@@ -6639,7 +6648,6 @@
         </is>
       </c>
     </row>
-    <row r="180"/>
     <row r="181">
       <c r="A181" s="9" t="inlineStr">
         <is>
@@ -6661,7 +6669,6 @@
         </is>
       </c>
     </row>
-    <row r="184"/>
     <row r="185">
       <c r="A185" s="26" t="inlineStr">
         <is>
@@ -6669,8 +6676,6 @@
         </is>
       </c>
     </row>
-    <row r="186"/>
-    <row r="187"/>
     <row r="188">
       <c r="A188" s="25" t="inlineStr">
         <is>
@@ -6678,7 +6683,6 @@
         </is>
       </c>
     </row>
-    <row r="189"/>
     <row r="190">
       <c r="A190" s="9" t="inlineStr">
         <is>
@@ -6700,7 +6704,6 @@
         </is>
       </c>
     </row>
-    <row r="193"/>
     <row r="194">
       <c r="A194" s="26" t="inlineStr">
         <is>
@@ -6708,8 +6711,6 @@
         </is>
       </c>
     </row>
-    <row r="195"/>
-    <row r="196"/>
     <row r="197">
       <c r="A197" s="25" t="inlineStr">
         <is>
@@ -6717,7 +6718,6 @@
         </is>
       </c>
     </row>
-    <row r="198"/>
     <row r="199">
       <c r="A199" s="9" t="inlineStr">
         <is>
@@ -6739,7 +6739,6 @@
         </is>
       </c>
     </row>
-    <row r="202"/>
     <row r="203">
       <c r="A203" s="26" t="inlineStr">
         <is>
@@ -6747,8 +6746,6 @@
         </is>
       </c>
     </row>
-    <row r="204"/>
-    <row r="205"/>
     <row r="206">
       <c r="A206" s="25" t="inlineStr">
         <is>
@@ -6756,7 +6753,6 @@
         </is>
       </c>
     </row>
-    <row r="207"/>
     <row r="208">
       <c r="A208" s="9" t="inlineStr">
         <is>
@@ -6778,7 +6774,6 @@
         </is>
       </c>
     </row>
-    <row r="211"/>
     <row r="212">
       <c r="A212" s="26" t="inlineStr">
         <is>
@@ -6786,8 +6781,6 @@
         </is>
       </c>
     </row>
-    <row r="213"/>
-    <row r="214"/>
     <row r="215">
       <c r="A215" s="25" t="inlineStr">
         <is>
@@ -6795,7 +6788,6 @@
         </is>
       </c>
     </row>
-    <row r="216"/>
     <row r="217">
       <c r="A217" s="9" t="inlineStr">
         <is>
@@ -6817,7 +6809,6 @@
         </is>
       </c>
     </row>
-    <row r="220"/>
     <row r="221">
       <c r="A221" s="26" t="inlineStr">
         <is>
@@ -6858,7 +6849,6 @@
       <c r="B1" s="2" t="inlineStr"/>
       <c r="C1" s="2" t="inlineStr"/>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7724,7 +7714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7788,106 +7778,103 @@
         </is>
       </c>
     </row>
-    <row r="10"/>
     <row r="11">
       <c r="A11" s="21" t="inlineStr">
         <is>
-          <t>10개 키 조합:</t>
+          <t>버전별 차이점:</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3-Key (가장 정밀): SEO, SEC, SOC, EOC</t>
+          <t>LIGHT 버전 동작:</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2-Key (덜 정밀): SE, SO, SC, EO, EC, OC</t>
-        </is>
-      </c>
-    </row>
-    <row r="14"/>
+          <t xml:space="preserve">  • 구두점/공백만 변경: "Punctuation/Space Change"</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 내용 변경: "Content Change"</t>
+        </is>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" s="21" t="inlineStr">
-        <is>
-          <t>왜 단순 룩업 대신 10개 조합을 사용하나요?</t>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>FULL 버전 동작 (BERT AI 포함):</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 중복 StrOrigin 처리 (예: 다른 캐릭터가 말하는 '안녕하세요')</t>
+      <c r="A16" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 구두점/공백만 변경: "Punctuation/Space Change"</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 빈 StrOrigin 셀 처리</t>
+          <t xml:space="preserve">  • 내용 변경: 유사도 백분율 (예: "94.5% similar", "48.2% similar")</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t xml:space="preserve">  2-Key (덜 정밀): SE, SO, SC, EO, EC, OC</t>
+        </is>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" s="21" t="inlineStr">
+        <is>
+          <t>왜 단순 룩업 대신 10개 조합을 사용하나요?</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 중복 StrOrigin 처리 (예: 다른 캐릭터가 말하는 '안녕하세요')</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 빈 StrOrigin 셀 처리</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t xml:space="preserve">  • EventName 변경 처리 (E가 변경되어도 SO 또는 OC 키로 여전히 매칭)</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t xml:space="preserve">  • 중복 CastingKey 처리 (같은 캐릭터가 여러 번 말하는 경우)</t>
         </is>
       </c>
     </row>
-    <row r="20"/>
-    <row r="21">
-      <c r="A21" s="4" t="inlineStr">
+    <row r="25"/>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
         <is>
           <t>색상 코딩 참조</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr"/>
-      <c r="C21" s="2" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr"/>
-      <c r="B22" s="2" t="inlineStr"/>
-      <c r="C22" s="2" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>모든 출력 파일은 변경 유형에 대해 일관된 색상 코딩을 사용합니다:</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr"/>
-      <c r="C23" s="2" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr"/>
-      <c r="B24" s="2" t="inlineStr"/>
-      <c r="C24" s="2" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>주황색 (FFD580) - StrOrigin Change</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr"/>
-      <c r="C25" s="2" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  한국어 원문이 변경되었습니다. 최우선순위 - 번역 업데이트가 필요할 가능성이 높음.</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr"/>
@@ -7899,189 +7886,193 @@
       <c r="C27" s="2" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>연보라색 (E1D5FF) - Desc Change</t>
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>모든 출력 파일은 변경 유형에 대해 일관된 색상 코딩을 사용합니다:</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr"/>
       <c r="C28" s="2" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  설명/맥락이 변경되었습니다. 업데이트된 맥락 정보를 검토하세요.</t>
-        </is>
-      </c>
+      <c r="A29" s="2" t="inlineStr"/>
       <c r="B29" s="2" t="inlineStr"/>
       <c r="C29" s="2" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr"/>
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>주황색 (FFD580) - StrOrigin Change</t>
+        </is>
+      </c>
       <c r="B30" s="2" t="inlineStr"/>
       <c r="C30" s="2" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>연한 빨강 (FF9999) - TimeFrame Change</t>
+          <t xml:space="preserve">  한국어 원문이 변경되었습니다. 최우선순위 - 번역 업데이트가 필요할 가능성이 높음.</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr"/>
       <c r="C31" s="2" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  타이밍이 조정되었습니다. 내용은 변경되지 않았으며 번역은 여전히 유효합니다.</t>
-        </is>
-      </c>
+      <c r="A32" s="2" t="inlineStr"/>
       <c r="B32" s="2" t="inlineStr"/>
       <c r="C32" s="2" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr"/>
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>연보라색 (E1D5FF) - Desc Change</t>
+        </is>
+      </c>
       <c r="B33" s="2" t="inlineStr"/>
       <c r="C33" s="2" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>노란색 (FFFF99) - EventName Change</t>
+          <t xml:space="preserve">  설명/맥락이 변경되었습니다. 업데이트된 맥락 정보를 검토하세요.</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr"/>
       <c r="C34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  이벤트 이름이 변경되었지만 한국어 텍스트는 동일합니다. 일반적으로 우선순위가 낮습니다.</t>
-        </is>
-      </c>
+      <c r="A35" s="2" t="inlineStr"/>
       <c r="B35" s="2" t="inlineStr"/>
       <c r="C35" s="2" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="inlineStr"/>
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>연한 빨강 (FF9999) - TimeFrame Change</t>
+        </is>
+      </c>
       <c r="B36" s="2" t="inlineStr"/>
       <c r="C36" s="2" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>하늘색 (87CEFA) - Character Group Change</t>
+          <t xml:space="preserve">  타이밍이 조정되었습니다. 내용은 변경되지 않았으며 번역은 여전히 유효합니다.</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr"/>
       <c r="C37" s="2" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  캐릭터 속성이 업데이트되었습니다. 캐스팅 및 보이스 디렉션에 중요합니다.</t>
-        </is>
-      </c>
+      <c r="A38" s="2" t="inlineStr"/>
       <c r="B38" s="2" t="inlineStr"/>
       <c r="C38" s="2" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr"/>
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>노란색 (FFFF99) - EventName Change</t>
+        </is>
+      </c>
       <c r="B39" s="2" t="inlineStr"/>
       <c r="C39" s="2" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>연두색 (90EE90) - New Row</t>
+          <t xml:space="preserve">  이벤트 이름이 변경되었지만 한국어 텍스트는 동일합니다. 일반적으로 우선순위가 낮습니다.</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr"/>
       <c r="C40" s="2" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  완전히 새로운 대사입니다. 새로운 번역이 필요합니다.</t>
-        </is>
-      </c>
+      <c r="A41" s="2" t="inlineStr"/>
       <c r="B41" s="2" t="inlineStr"/>
       <c r="C41" s="2" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="inlineStr"/>
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>하늘색 (87CEFA) - Character Group Change</t>
+        </is>
+      </c>
       <c r="B42" s="2" t="inlineStr"/>
       <c r="C42" s="2" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>연한 회색 (D3D3D3) - No Relevant Change</t>
+          <t xml:space="preserve">  캐릭터 속성이 업데이트되었습니다. 캐스팅 및 보이스 디렉션에 중요합니다.</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr"/>
       <c r="C43" s="2" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  사소한 변경만 있습니다. 우선순위가 낮은 검토.</t>
-        </is>
-      </c>
+      <c r="A44" s="2" t="inlineStr"/>
       <c r="B44" s="2" t="inlineStr"/>
       <c r="C44" s="2" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr"/>
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>연두색 (90EE90) - New Row</t>
+        </is>
+      </c>
       <c r="B45" s="2" t="inlineStr"/>
       <c r="C45" s="2" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>매우 연한 회색 (E8E8E8) - No Change</t>
+          <t xml:space="preserve">  완전히 새로운 대사입니다. 새로운 번역이 필요합니다.</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr"/>
       <c r="C46" s="2" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  완전히 동일합니다. 조치가 필요하지 않습니다.</t>
-        </is>
-      </c>
+      <c r="A47" s="2" t="inlineStr"/>
       <c r="B47" s="2" t="inlineStr"/>
       <c r="C47" s="2" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="inlineStr"/>
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>연한 회색 (D3D3D3) - No Relevant Change</t>
+        </is>
+      </c>
       <c r="B48" s="2" t="inlineStr"/>
       <c r="C48" s="2" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr"/>
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  사소한 변경만 있습니다. 우선순위가 낮은 검토.</t>
+        </is>
+      </c>
       <c r="B49" s="2" t="inlineStr"/>
       <c r="C49" s="2" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="inlineStr">
-        <is>
-          <t>STATUS 색상 코딩</t>
-        </is>
-      </c>
+      <c r="A50" s="2" t="inlineStr"/>
       <c r="B50" s="2" t="inlineStr"/>
       <c r="C50" s="2" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="inlineStr"/>
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>매우 연한 회색 (E8E8E8) - No Change</t>
+        </is>
+      </c>
       <c r="B51" s="2" t="inlineStr"/>
       <c r="C51" s="2" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="inlineStr">
-        <is>
-          <t>STATUS 값도 빠른 시각적 스캔을 위해 색상 코딩됩니다:</t>
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  완전히 동일합니다. 조치가 필요하지 않습니다.</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr"/>
@@ -8093,50 +8084,42 @@
       <c r="C53" s="2" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="inlineStr">
-        <is>
-          <t>연두색 (90EE90)</t>
-        </is>
-      </c>
+      <c r="A54" s="2" t="inlineStr"/>
       <c r="B54" s="2" t="inlineStr"/>
       <c r="C54" s="2" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  RECORDED, 녹음 완료, 已录音</t>
+      <c r="A55" s="4" t="inlineStr">
+        <is>
+          <t>STATUS 색상 코딩</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr"/>
       <c r="C55" s="2" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  녹음 완료 - 작업이 완료됨</t>
-        </is>
-      </c>
+      <c r="A56" s="2" t="inlineStr"/>
       <c r="B56" s="2" t="inlineStr"/>
       <c r="C56" s="2" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="inlineStr"/>
+      <c r="A57" s="5" t="inlineStr">
+        <is>
+          <t>STATUS 값도 빠른 시각적 스캔을 위해 색상 코딩됩니다:</t>
+        </is>
+      </c>
       <c r="B57" s="2" t="inlineStr"/>
       <c r="C57" s="2" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="inlineStr">
-        <is>
-          <t>연보라색 (E6D5FF)</t>
-        </is>
-      </c>
+      <c r="A58" s="2" t="inlineStr"/>
       <c r="B58" s="2" t="inlineStr"/>
       <c r="C58" s="2" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  POLISHED, 준비 중, 准备中</t>
+          <t>연두색 (90EE90)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr"/>
@@ -8145,30 +8128,30 @@
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  텍스트가 다듬어짐, 녹음 준비 완료</t>
+          <t xml:space="preserve">  RECORDED, 녹음 완료, 已录音</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr"/>
       <c r="C60" s="2" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="inlineStr"/>
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  녹음 완료 - 작업이 완료됨</t>
+        </is>
+      </c>
       <c r="B61" s="2" t="inlineStr"/>
       <c r="C61" s="2" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="inlineStr">
-        <is>
-          <t>연한 빨강 (FFB3B3)</t>
-        </is>
-      </c>
+      <c r="A62" s="2" t="inlineStr"/>
       <c r="B62" s="2" t="inlineStr"/>
       <c r="C62" s="2" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  RE-RECORD, NEED CHECK, 재녹음 필요, 需补录</t>
+          <t>연보라색 (E6D5FF)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr"/>
@@ -8177,30 +8160,30 @@
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  주의가 필요하거나 재녹음이 필요함</t>
+          <t xml:space="preserve">  POLISHED, 준비 중, 准备中</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr"/>
       <c r="C64" s="2" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="inlineStr"/>
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  텍스트가 다듬어짐, 녹음 준비 완료</t>
+        </is>
+      </c>
       <c r="B65" s="2" t="inlineStr"/>
       <c r="C65" s="2" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="inlineStr">
-        <is>
-          <t>연한 초록 (C5E8C5)</t>
-        </is>
-      </c>
+      <c r="A66" s="2" t="inlineStr"/>
       <c r="B66" s="2" t="inlineStr"/>
       <c r="C66" s="2" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  RE-RECORDED, 재녹음 완료, 已补录</t>
+          <t>연한 빨강 (FFB3B3)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr"/>
@@ -8209,30 +8192,30 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  재녹음 완료</t>
+          <t xml:space="preserve">  RE-RECORD, NEED CHECK, 재녹음 필요, 需补录</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr"/>
       <c r="C68" s="2" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="inlineStr"/>
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  주의가 필요하거나 재녹음이 필요함</t>
+        </is>
+      </c>
       <c r="B69" s="2" t="inlineStr"/>
       <c r="C69" s="2" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="inlineStr">
-        <is>
-          <t>연한 노랑 (FFFFE0)</t>
-        </is>
-      </c>
+      <c r="A70" s="2" t="inlineStr"/>
       <c r="B70" s="2" t="inlineStr"/>
       <c r="C70" s="2" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PREVIOUSLY RECORDED, 전달 완료, 已传达</t>
+          <t>연한 초록 (C5E8C5)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr"/>
@@ -8241,30 +8224,30 @@
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  이전에 전달/녹음됨</t>
+          <t xml:space="preserve">  RE-RECORDED, 재녹음 완료, 已补录</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr"/>
       <c r="C72" s="2" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="inlineStr"/>
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  재녹음 완료</t>
+        </is>
+      </c>
       <c r="B73" s="2" t="inlineStr"/>
       <c r="C73" s="2" t="inlineStr"/>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="inlineStr">
-        <is>
-          <t>하늘색 (87CEEB)</t>
-        </is>
-      </c>
+      <c r="A74" s="2" t="inlineStr"/>
       <c r="B74" s="2" t="inlineStr"/>
       <c r="C74" s="2" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  FINAL, SHIPPED</t>
+          <t>연한 노랑 (FFFFE0)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr"/>
@@ -8273,14 +8256,18 @@
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  최종 완료 및 전달됨</t>
+          <t xml:space="preserve">  PREVIOUSLY RECORDED, 전달 완료, 已传达</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr"/>
       <c r="C76" s="2" t="inlineStr"/>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="inlineStr"/>
+      <c r="A77" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  이전에 전달/녹음됨</t>
+        </is>
+      </c>
       <c r="B77" s="2" t="inlineStr"/>
       <c r="C77" s="2" t="inlineStr"/>
     </row>
@@ -8290,23 +8277,27 @@
       <c r="C78" s="2" t="inlineStr"/>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="inlineStr">
-        <is>
-          <t>업데이트 히스토리 시스템</t>
+      <c r="A79" s="2" t="inlineStr">
+        <is>
+          <t>하늘색 (87CEEB)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr"/>
       <c r="C79" s="2" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="inlineStr"/>
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  FINAL, SHIPPED</t>
+        </is>
+      </c>
       <c r="B80" s="2" t="inlineStr"/>
       <c r="C80" s="2" t="inlineStr"/>
     </row>
     <row r="81">
-      <c r="A81" s="5" t="inlineStr">
-        <is>
-          <t>VRS Manager는 JSON 파일로 모든 프로세스 실행을 추적합니다:</t>
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  최종 완료 및 전달됨</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr"/>
@@ -8318,18 +8309,14 @@
       <c r="C82" s="2" t="inlineStr"/>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="inlineStr">
-        <is>
-          <t>working_update_history.json</t>
-        </is>
-      </c>
+      <c r="A83" s="2" t="inlineStr"/>
       <c r="B83" s="2" t="inlineStr"/>
       <c r="C83" s="2" t="inlineStr"/>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  모든 Working Process 실행 기록</t>
+      <c r="A84" s="4" t="inlineStr">
+        <is>
+          <t>업데이트 히스토리 시스템</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr"/>
@@ -8341,82 +8328,78 @@
       <c r="C85" s="2" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="inlineStr">
-        <is>
-          <t>alllang_update_history.json</t>
+      <c r="A86" s="5" t="inlineStr">
+        <is>
+          <t>VRS Manager는 JSON 파일로 모든 프로세스 실행을 추적합니다:</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr"/>
       <c r="C86" s="2" t="inlineStr"/>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  모든 All Language Process 실행 기록</t>
-        </is>
-      </c>
+      <c r="A87" s="2" t="inlineStr"/>
       <c r="B87" s="2" t="inlineStr"/>
       <c r="C87" s="2" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  어떤 언어가 업데이트되고 보존되었는지 포함</t>
+          <t>working_update_history.json</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr"/>
       <c r="C88" s="2" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="inlineStr"/>
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  모든 Working Process 실행 기록</t>
+        </is>
+      </c>
       <c r="B89" s="2" t="inlineStr"/>
       <c r="C89" s="2" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="inlineStr">
-        <is>
-          <t>master_update_history.json</t>
-        </is>
-      </c>
+      <c r="A90" s="2" t="inlineStr"/>
       <c r="B90" s="2" t="inlineStr"/>
       <c r="C90" s="2" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  모든 Master File Update 실행 기록</t>
+          <t>alllang_update_history.json</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr"/>
       <c r="C91" s="2" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="inlineStr"/>
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  모든 All Language Process 실행 기록</t>
+        </is>
+      </c>
       <c r="B92" s="2" t="inlineStr"/>
       <c r="C92" s="2" t="inlineStr"/>
     </row>
     <row r="93">
-      <c r="A93" s="5" t="inlineStr">
-        <is>
-          <t>각 레코드에 포함된 것:</t>
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  어떤 언어가 업데이트되고 보존되었는지 포함</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr"/>
       <c r="C93" s="2" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 실행 타임스탬프</t>
-        </is>
-      </c>
+      <c r="A94" s="2" t="inlineStr"/>
       <c r="B94" s="2" t="inlineStr"/>
       <c r="C94" s="2" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 입력 파일명</t>
+          <t>master_update_history.json</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr"/>
@@ -8425,25 +8408,21 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 출력 파일명</t>
+          <t xml:space="preserve">  모든 Master File Update 실행 기록</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr"/>
       <c r="C96" s="2" t="inlineStr"/>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 변경에 대한 상세 통계</t>
-        </is>
-      </c>
+      <c r="A97" s="2" t="inlineStr"/>
       <c r="B97" s="2" t="inlineStr"/>
       <c r="C97" s="2" t="inlineStr"/>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 카테고리별 단어 수</t>
+      <c r="A98" s="5" t="inlineStr">
+        <is>
+          <t>각 레코드에 포함된 것:</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr"/>
@@ -8452,21 +8431,25 @@
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 언어 업데이트 상태 (All Language만)</t>
+          <t xml:space="preserve">  • 실행 타임스탬프</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr"/>
       <c r="C99" s="2" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="inlineStr"/>
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 입력 파일명</t>
+        </is>
+      </c>
       <c r="B100" s="2" t="inlineStr"/>
       <c r="C100" s="2" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" s="5" t="inlineStr">
-        <is>
-          <t>GUI를 통한 접근:</t>
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 출력 파일명</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr"/>
@@ -8475,7 +8458,7 @@
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  메인 창의 'View Update History' 버튼 클릭</t>
+          <t xml:space="preserve">  • 변경에 대한 상세 통계</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr"/>
@@ -8484,7 +8467,7 @@
     <row r="103">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  보려는 프로세스 유형 선택 (Master / All Language / Working)</t>
+          <t xml:space="preserve">  • 카테고리별 단어 수</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr"/>
@@ -8493,7 +8476,7 @@
     <row r="104">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  완전한 세부정보와 함께 포맷된 히스토리 보기</t>
+          <t xml:space="preserve">  • 언어 업데이트 상태 (All Language만)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr"/>
@@ -8505,39 +8488,43 @@
       <c r="C105" s="2" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="inlineStr"/>
+      <c r="A106" s="5" t="inlineStr">
+        <is>
+          <t>GUI를 통한 접근:</t>
+        </is>
+      </c>
       <c r="B106" s="2" t="inlineStr"/>
       <c r="C106" s="2" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" s="4" t="inlineStr">
-        <is>
-          <t>버전 정보</t>
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  메인 창의 'View Update History' 버튼 클릭</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr"/>
       <c r="C107" s="2" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="inlineStr"/>
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  보려는 프로세스 유형 선택 (Master / All Language / Working)</t>
+        </is>
+      </c>
       <c r="B108" s="2" t="inlineStr"/>
       <c r="C108" s="2" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>현재 버전: 1113</t>
+          <t xml:space="preserve">  완전한 세부정보와 함께 포맷된 히스토리 보기</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr"/>
       <c r="C109" s="2" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="inlineStr">
-        <is>
-          <t>릴리스 날짜: 2024년 11월</t>
-        </is>
-      </c>
+      <c r="A110" s="2" t="inlineStr"/>
       <c r="B110" s="2" t="inlineStr"/>
       <c r="C110" s="2" t="inlineStr"/>
     </row>
@@ -8547,27 +8534,23 @@
       <c r="C111" s="2" t="inlineStr"/>
     </row>
     <row r="112">
-      <c r="A112" s="5" t="inlineStr">
-        <is>
-          <t>버전 1113의 주요 개선사항:</t>
+      <c r="A112" s="4" t="inlineStr">
+        <is>
+          <t>버전 정보</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr"/>
       <c r="C112" s="2" t="inlineStr"/>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 단순화된 Master File Update 로직</t>
-        </is>
-      </c>
+      <c r="A113" s="2" t="inlineStr"/>
       <c r="B113" s="2" t="inlineStr"/>
       <c r="C113" s="2" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 셀별 비교 대신 빠른 복사-붙여넣기 처리</t>
+          <t>현재 버전: 1113</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr"/>
@@ -8576,25 +8559,21 @@
     <row r="115">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 특정 예외 규칙을 사용한 향상된 TimeFrame 보존</t>
+          <t>릴리스 날짜: 2024년 11월</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr"/>
       <c r="C115" s="2" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • 유연한 업데이트가 가능한 개선된 다국어 지원</t>
-        </is>
-      </c>
+      <c r="A116" s="2" t="inlineStr"/>
       <c r="B116" s="2" t="inlineStr"/>
       <c r="C116" s="2" t="inlineStr"/>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  • JSON 저장을 사용한 포괄적인 업데이트 히스토리 추적</t>
+      <c r="A117" s="5" t="inlineStr">
+        <is>
+          <t>버전 1113의 주요 개선사항:</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr"/>
@@ -8603,432 +8582,448 @@
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 시각적 명확성을 위한 더 나은 색상 코딩 시스템</t>
+          <t xml:space="preserve">  • 단순화된 Master File Update 로직</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr"/>
       <c r="C118" s="2" t="inlineStr"/>
     </row>
-    <row r="119"/>
-    <row r="120"/>
+    <row r="119">
+      <c r="A119" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 셀별 비교 대신 빠른 복사-붙여넣기 처리</t>
+        </is>
+      </c>
+      <c r="B119" s="2" t="inlineStr"/>
+      <c r="C119" s="2" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 특정 예외 규칙을 사용한 향상된 TimeFrame 보존</t>
+        </is>
+      </c>
+      <c r="B120" s="2" t="inlineStr"/>
+      <c r="C120" s="2" t="inlineStr"/>
+    </row>
     <row r="121">
-      <c r="A121" s="10" t="inlineStr">
+      <c r="A121" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 유연한 업데이트가 가능한 개선된 다국어 지원</t>
+        </is>
+      </c>
+      <c r="B121" s="2" t="inlineStr"/>
+      <c r="C121" s="2" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • JSON 저장을 사용한 포괄적인 업데이트 히스토리 추적</t>
+        </is>
+      </c>
+      <c r="B122" s="2" t="inlineStr"/>
+      <c r="C122" s="2" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 시각적 명확성을 위한 더 나은 색상 코딩 시스템</t>
+        </is>
+      </c>
+      <c r="B123" s="2" t="inlineStr"/>
+      <c r="C123" s="2" t="inlineStr"/>
+    </row>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126">
+      <c r="A126" s="10" t="inlineStr">
         <is>
           <t>TWO-PASS 알고리즘 (v1116)</t>
         </is>
       </c>
     </row>
-    <row r="122"/>
-    <row r="123">
-      <c r="A123" s="9" t="inlineStr">
+    <row r="127"/>
+    <row r="128">
+      <c r="A128" s="9" t="inlineStr">
         <is>
           <t>PASS 1 - 확실한 항목 감지 및 마킹:</t>
         </is>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
+    <row r="129">
+      <c r="A129" t="inlineStr">
         <is>
           <t>1. 모든 CURRENT 행 처리</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>2. 완벽한 매치 (모든 10개 키 매치) → "No Change" → PREVIOUS 행 마킹</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>3. 매치 없음 (모든 10개 키 누락) → "New Row"</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → "Deleted"</t>
-        </is>
-      </c>
-    </row>
-    <row r="128"/>
-    <row r="129">
-      <c r="A129" s="9" t="inlineStr">
-        <is>
-          <t>PASS 2 - 변경 감지:</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+          <t>2. 완벽한 매치 (모든 10개 키 매치) → "No Change" → PREVIOUS 행 마킹</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
+          <t>3. 매치 없음 (모든 10개 키 누락) → "New Row"</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>3. 마크되지 않은 PREVIOUS 행만 사용</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
-        </is>
-      </c>
-    </row>
+          <t>4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → "Deleted"</t>
+        </is>
+      </c>
+    </row>
+    <row r="133"/>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>5. 마크되지 않은 매치 없음 → "New Row"</t>
-        </is>
-      </c>
-    </row>
-    <row r="135"/>
+      <c r="A134" s="9" t="inlineStr">
+        <is>
+          <t>PASS 2 - 변경 감지:</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+        </is>
+      </c>
+    </row>
     <row r="136">
-      <c r="A136" s="9" t="inlineStr">
-        <is>
-          <t>왜 이것이 작동하는가:</t>
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>• PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
+          <t>3. 마크되지 않은 PREVIOUS 행만 사용</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>• PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
+          <t>4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>5. 마크되지 않은 매치 없음 → "New Row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="140"/>
+    <row r="141">
+      <c r="A141" s="9" t="inlineStr">
+        <is>
+          <t>왜 이것이 작동하는가:</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>• PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>• PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
           <t>• 모든 엣지 케이스 처리: 중복 StrOrigin, 빈 셀, 중복 CastingKey</t>
         </is>
       </c>
     </row>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142">
-      <c r="A142" s="10" t="inlineStr">
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147">
+      <c r="A147" s="10" t="inlineStr">
         <is>
           <t>TWO-PASS 알고리즘 (v1116)</t>
         </is>
       </c>
     </row>
-    <row r="143"/>
-    <row r="144">
-      <c r="A144" s="9" t="inlineStr">
+    <row r="148"/>
+    <row r="149">
+      <c r="A149" s="9" t="inlineStr">
         <is>
           <t>PASS 1 - 확실한 항목 감지 및 마킹:</t>
         </is>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
+    <row r="150">
+      <c r="A150" t="inlineStr">
         <is>
           <t>1. 모든 CURRENT 행 처리</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>2. 완벽한 매치 (모든 10개 키 매치) → "No Change" → PREVIOUS 행 마킹</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>3. 매치 없음 (모든 10개 키 누락) → "New Row"</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → "Deleted"</t>
-        </is>
-      </c>
-    </row>
-    <row r="149"/>
-    <row r="150">
-      <c r="A150" s="9" t="inlineStr">
-        <is>
-          <t>PASS 2 - 변경 감지:</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+          <t>2. 완벽한 매치 (모든 10개 키 매치) → "No Change" → PREVIOUS 행 마킹</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
+          <t>3. 매치 없음 (모든 10개 키 누락) → "New Row"</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>3. 마크되지 않은 PREVIOUS 행만 사용</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
-        </is>
-      </c>
-    </row>
+          <t>4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → "Deleted"</t>
+        </is>
+      </c>
+    </row>
+    <row r="154"/>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>5. 마크되지 않은 매치 없음 → "New Row"</t>
-        </is>
-      </c>
-    </row>
-    <row r="156"/>
+      <c r="A155" s="9" t="inlineStr">
+        <is>
+          <t>PASS 2 - 변경 감지:</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+        </is>
+      </c>
+    </row>
     <row r="157">
-      <c r="A157" s="9" t="inlineStr">
-        <is>
-          <t>왜 이것이 작동하는가:</t>
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>• PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
+          <t>3. 마크되지 않은 PREVIOUS 행만 사용</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>• PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
+          <t>4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>• 모든 엣지 케이스 처리: 중복 StrOrigin, 빈 셀, 중복 CastingKey</t>
+          <t>5. 마크되지 않은 매치 없음 → "New Row"</t>
         </is>
       </c>
     </row>
     <row r="161"/>
     <row r="162">
-      <c r="A162" s="14" t="inlineStr">
-        <is>
-          <t>TWO-PASS 알고리즘 (v1116)</t>
+      <c r="A162" s="9" t="inlineStr">
+        <is>
+          <t>왜 이것이 작동하는가:</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>TWO-PASS 알고리즘은 PREVIOUS의 각 행이 CURRENT의 최대 한 행과만 매칭되도록 보장하여</t>
+          <t>• PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>이전 버전에서 발생했던 1-to-many 매칭 문제를 방지합니다.</t>
-        </is>
-      </c>
-    </row>
-    <row r="165"/>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>PASS 1 - 확실한 항목 감지 및 마킹:</t>
-        </is>
-      </c>
-    </row>
+          <t>• PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>• 모든 엣지 케이스 처리: 중복 StrOrigin, 빈 셀, 중복 CastingKey</t>
+        </is>
+      </c>
+    </row>
+    <row r="166"/>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  1. 모든 CURRENT 행 처리</t>
+      <c r="A167" s="14" t="inlineStr">
+        <is>
+          <t>TWO-PASS 알고리즘 (v1116)</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2. 완벽한 매치 (모든 10개 키 매치) → 'No Change' → PREVIOUS 행 마킹</t>
+          <t>TWO-PASS 알고리즘은 PREVIOUS의 각 행이 CURRENT의 최대 한 행과만 매칭되도록 보장하여</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3. 매치 없음 (모든 10개 키 누락) → 'New Row'</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → 'Deleted'</t>
-        </is>
-      </c>
-    </row>
-    <row r="171"/>
+          <t>이전 버전에서 발생했던 1-to-many 매칭 문제를 방지합니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="170"/>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>PASS 1 - 확실한 항목 감지 및 마킹:</t>
+        </is>
+      </c>
+    </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>PASS 2 - 변경 감지:</t>
+          <t xml:space="preserve">  1. 모든 CURRENT 행 처리</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+          <t xml:space="preserve">  2. 완벽한 매치 (모든 10개 키 매치) → 'No Change' → PREVIOUS 행 마킹</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
+          <t xml:space="preserve">  3. 매치 없음 (모든 10개 키 누락) → 'New Row'</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3. 마크되지 않은 PREVIOUS 행만 사용</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
-        </is>
-      </c>
-    </row>
+          <t xml:space="preserve">  4. 모든 CURRENT 처리 후: 마크되지 않은 PREVIOUS 행 → 'Deleted'</t>
+        </is>
+      </c>
+    </row>
+    <row r="176"/>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5. 마크되지 않은 매치 없음 → 'New Row'</t>
-        </is>
-      </c>
-    </row>
-    <row r="178"/>
+          <t>PASS 2 - 변경 감지:</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1. PASS 1에서 분류되지 않은 CURRENT 행 처리</t>
+        </is>
+      </c>
+    </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>왜 이것이 작동하는가:</t>
+          <t xml:space="preserve">  2. 10개 키로 패턴 매칭 (3-key 먼저, 그 다음 2-key)</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
+          <t xml:space="preserve">  3. 마크되지 않은 PREVIOUS 행만 사용</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
+          <t xml:space="preserve">  4. 첫 번째 마크되지 않은 매치 우선 (결정론적)</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 모든 엣지 케이스 처리: 중복 StrOrigin, 빈 셀, 중복 CastingKey</t>
+          <t xml:space="preserve">  5. 마크되지 않은 매치 없음 → 'New Row'</t>
         </is>
       </c>
     </row>
     <row r="183"/>
     <row r="184">
-      <c r="A184" s="9" t="inlineStr">
-        <is>
-          <t>예제: 중복 STRORIGIN 처리</t>
-        </is>
-      </c>
-    </row>
-    <row r="185"/>
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>왜 이것이 작동하는가:</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - PASS 1이 확실한 항목을 마킹하여 재사용 방지</t>
+        </is>
+      </c>
+    </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>시나리오:</t>
+          <t xml:space="preserve">  - PASS 2는 마크되지 않은 행만 사용하여 1-to-1 매칭 보장</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PREVIOUS 파일에 공통 문구 "안녕하세요"가 있는 1개 행</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  CURRENT 파일에 "안녕하세요"가 있는 3개 행 (1개는 같은 캐릭터, 2개는 다른 캐릭터)</t>
-        </is>
-      </c>
-    </row>
-    <row r="189"/>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>이전 (v1114v4 - 문제):</t>
-        </is>
-      </c>
-    </row>
+          <t xml:space="preserve">  - 모든 엣지 케이스 처리: 중복 StrOrigin, 빈 셀, 중복 CastingKey</t>
+        </is>
+      </c>
+    </row>
+    <row r="188"/>
+    <row r="189">
+      <c r="A189" s="9" t="inlineStr">
+        <is>
+          <t>예제: 중복 STRORIGIN 처리</t>
+        </is>
+      </c>
+    </row>
+    <row r="190"/>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 1개 PREVIOUS 행이 모든 3개 CURRENT 행과 매칭</t>
+          <t>시나리오:</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 결과: 2개 행이 "New Row" 대신 "EventName Change"로 잘못 표시됨</t>
+          <t xml:space="preserve">  PREVIOUS 파일에 공통 문구 "안녕하세요"가 있는 1개 행</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - 행 계산 수학: 문제 (new_rows - deleted_rows ≠ actual_difference)</t>
+          <t xml:space="preserve">  CURRENT 파일에 "안녕하세요"가 있는 3개 행 (1개는 같은 캐릭터, 2개는 다른 캐릭터)</t>
         </is>
       </c>
     </row>
@@ -9036,33 +9031,62 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>이후 (v1116 - TWO-PASS로 수정):</t>
+          <t>이전 (v1114v4 - 문제):</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - PASS 1: 완벽한 매치 발견 → 1개 CURRENT 행 "No Change" 표시, PREVIOUS 행 마킹</t>
+          <t xml:space="preserve">  - 1개 PREVIOUS 행이 모든 3개 CURRENT 행과 매칭</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - PASS 2: 나머지 2개 CURRENT 행 → 마크되지 않은 PREVIOUS 매치 없음 → "New Row"</t>
+          <t xml:space="preserve">  - 결과: 2개 행이 "New Row" 대신 "EventName Change"로 잘못 표시됨</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
+          <t xml:space="preserve">  - 행 계산 수학: 문제 (new_rows - deleted_rows ≠ actual_difference)</t>
+        </is>
+      </c>
+    </row>
+    <row r="199"/>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>이후 (v1116 - TWO-PASS로 수정):</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - PASS 1: 완벽한 매치 발견 → 1개 CURRENT 행 "No Change" 표시, PREVIOUS 행 마킹</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - PASS 2: 나머지 2개 CURRENT 행 → 마크되지 않은 PREVIOUS 매치 없음 → "New Row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
           <t xml:space="preserve">  - 결과: 올바른 분류 (1개 No Change, 2개 New Row)</t>
         </is>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
+    <row r="204">
+      <c r="A204" t="inlineStr">
         <is>
           <t xml:space="preserve">  - 행 계산 수학: 정확 (new_rows - deleted_rows = actual_difference) ✅</t>
         </is>
@@ -9079,7 +9103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B93"/>
+  <dimension ref="A4:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9092,9 +9116,6 @@
     <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="27" t="inlineStr">
         <is>
@@ -9102,7 +9123,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
@@ -9134,7 +9154,6 @@
         </is>
       </c>
     </row>
-    <row r="9"/>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
@@ -9250,7 +9269,6 @@
         </is>
       </c>
     </row>
-    <row r="20"/>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
@@ -9426,7 +9444,6 @@
         </is>
       </c>
     </row>
-    <row r="36"/>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
@@ -9470,7 +9487,6 @@
         </is>
       </c>
     </row>
-    <row r="41"/>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
@@ -9513,8 +9529,6 @@
         </is>
       </c>
     </row>
-    <row r="48"/>
-    <row r="49"/>
     <row r="50">
       <c r="A50" s="27" t="inlineStr">
         <is>
@@ -9522,7 +9536,6 @@
         </is>
       </c>
     </row>
-    <row r="51"/>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
@@ -9554,7 +9567,6 @@
         </is>
       </c>
     </row>
-    <row r="55"/>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
@@ -9670,7 +9682,6 @@
         </is>
       </c>
     </row>
-    <row r="66"/>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
@@ -9846,7 +9857,6 @@
         </is>
       </c>
     </row>
-    <row r="82"/>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
@@ -9890,7 +9900,6 @@
         </is>
       </c>
     </row>
-    <row r="87"/>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>

</xml_diff>